<commit_message>
recontructing the genus-protein-site relationships
</commit_message>
<xml_diff>
--- a/data/combined_markers.xlsx
+++ b/data/combined_markers.xlsx
@@ -508,12 +508,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['lipid biosynthesis proteins', 'fatty acid biosynthesis', 'biotin']</t>
+          <t>['biotin', 'fatty acid biosynthesis', 'lipid biosynthesis proteins']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -531,7 +531,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['site_8', 'site_8', 'site_11', 'site_6', 'site_1', 'site_4', 'site_11', 'site_4', 'site_1', 'site_1', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_11', 'site_6', 'site_1', 'site_4']</t>
         </is>
       </c>
     </row>
@@ -554,12 +554,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['lipid biosynthesis proteins', 'fatty acid biosynthesis']</t>
+          <t>['fatty acid biosynthesis', 'lipid biosynthesis proteins']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -577,7 +577,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['site_8', 'site_8', 'site_11', 'site_4', 'site_1', 'site_1', 'site_4', 'site_1', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_11', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -600,12 +600,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['lipid biosynthesis proteins', 'fatty acid biosynthesis', 'biotin']</t>
+          <t>['biotin', 'fatty acid biosynthesis', 'lipid biosynthesis proteins']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -623,7 +623,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['site_8', 'site_8', 'site_20', 'site_11', 'site_4', 'site_1', 'site_1', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_20', 'site_11', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -646,7 +646,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['site_8', 'site_6', 'site_11', 'site_4', 'site_1', 'site_11', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_6', 'site_11', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -692,7 +692,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -707,7 +707,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -715,7 +715,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['site_11', 'site_11', 'site_1', 'site_1', 'site_4', 'site_1', 'site_1', 'site_4']</t>
+          <t>['site_11', 'site_1', 'site_4']</t>
         </is>
       </c>
     </row>
@@ -738,7 +738,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['site_11', 'site_4', 'site_1', 'site_1', 'site_11', 'site_1', 'site_1']</t>
+          <t>['site_11', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -799,7 +799,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -807,7 +807,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['site_8', 'site_11', 'site_4', 'site_1', 'site_11', 'site_1']</t>
+          <t>['site_8', 'site_11', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -830,12 +830,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['carbon fixation by calvin cycle', 'alanine, aspartate and glutamate', 'phenylalanine', 'amino acid related enzymes', 'isoquinoline alkaloid biosynthesis', 'cysteine and methionine', 'novobiocin biosynthesis', 'phenylalanine, tyrosine and', 'tropane, piperidine and pyridine alkaloid biosynthesis, exosome', 'arginine and proline', 'tyrosine']</t>
+          <t>['alanine, aspartate and glutamate', 'phenylalanine, tyrosine and', 'novobiocin biosynthesis', 'carbon fixation by calvin cycle', 'amino acid related enzymes', 'arginine and proline', 'cysteine and methionine', 'isoquinoline alkaloid biosynthesis', 'tyrosine', 'tropane, piperidine and pyridine alkaloid biosynthesis, exosome', 'phenylalanine']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet', 'carbon_metabolism']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'carbon_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -853,7 +853,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['site_8', 'site_8', 'site_4', 'site_6', 'site_4', 'site_1']</t>
+          <t>['site_8', 'site_4', 'site_6', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -899,7 +899,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1', 'site_11', 'site_1', 'site_1', 'site_6']</t>
+          <t>['site_1', 'site_11', 'site_6']</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -937,7 +937,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['site_8', 'site_4', 'site_1', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -991,7 +991,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['site_8', 'site_6', 'site_1', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_6', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['site_6', 'site_1', 'site_1', 'site_1', 'site_11']</t>
+          <t>['site_6', 'site_1', 'site_11']</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['site_8', 'site_4', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_4', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1', 'site_1', 'site_1', 'site_11']</t>
+          <t>['site_1', 'site_11']</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['site_11', 'site_6', 'site_1', 'site_1']</t>
+          <t>['site_11', 'site_6', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['site_11', 'site_11', 'site_1', 'site_1']</t>
+          <t>['site_11', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['site_2', 'site_1', 'site_1', 'site_24']</t>
+          <t>['site_2', 'site_1', 'site_24']</t>
         </is>
       </c>
     </row>
@@ -1290,12 +1290,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['Mitochondrial biogenesis [BR:ko03029]', 'Viral proteins [BR:ko03200]', 'DNA repair and recombination proteins [BR:ko03400]', 'DNA replication proteins [BR:ko03032]']</t>
+          <t>['DNA repair and recombination proteins [BR:ko03400]', 'Mitochondrial biogenesis [BR:ko03029]', 'Viral proteins [BR:ko03200]', 'DNA replication proteins [BR:ko03032]']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'direct_eet']</t>
+          <t>['direct_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>['site_40', 'site_11', 'site_11', 'site_5']</t>
+          <t>['site_40', 'site_11', 'site_5']</t>
         </is>
       </c>
     </row>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1428,12 +1428,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['fluorobenzoate degradation', 'fatty acid degradation', 'dioxin degradation', 'toluene degradation', 'polycyclic aromatic hydrocarbon degradation', 'benzoate degradation', 'xylene degradation', 'chloroalkane and chloroalkene degradation']</t>
+          <t>['fluorobenzoate degradation', 'polycyclic aromatic hydrocarbon degradation', 'dioxin degradation', 'chloroalkane and chloroalkene degradation', 'toluene degradation', 'xylene degradation', 'fatty acid degradation', 'benzoate degradation']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['site_8', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['site_8', 'site_1', 'site_1', 'site_1']</t>
+          <t>['site_8', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['site_11', 'site_1', 'site_1']</t>
+          <t>['site_11', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1566,12 +1566,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['phenylalanine', 'isoquinoline alkaloid biosynthesis', 'cysteine and methionine', 'novobiocin biosynthesis', 'phenylalanine, tyrosine and', 'tropane, piperidine and pyridine alkaloid biosynthesis, amino acid related enzymes', 'ubiquinone and other terpenoid-quinone biosynthesis', 'tyrosine']</t>
+          <t>['phenylalanine, tyrosine and', 'tropane, piperidine and pyridine alkaloid biosynthesis, amino acid related enzymes', 'novobiocin biosynthesis', 'ubiquinone and other terpenoid-quinone biosynthesis', 'isoquinoline alkaloid biosynthesis', 'cysteine and methionine', 'tyrosine', 'phenylalanine']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['site_12', 'site_3', 'site_3']</t>
+          <t>['site_12', 'site_3']</t>
         </is>
       </c>
     </row>
@@ -1612,12 +1612,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['lipid biosynthesis proteins', 'fatty acid biosynthesis']</t>
+          <t>['fatty acid biosynthesis', 'lipid biosynthesis proteins']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'metal binding / chelation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'metal binding / chelation', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'metal_chelation', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'metal_chelation', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1', 'site_24']</t>
+          <t>['site_1', 'site_24']</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['site_1', 'site_11', 'site_1']</t>
+          <t>['site_1', 'site_11']</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['site_11', 'site_11', 'site_4']</t>
+          <t>['site_11', 'site_4']</t>
         </is>
       </c>
     </row>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -1934,7 +1934,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['site_40', 'site_1', 'site_1']</t>
+          <t>['site_40', 'site_1']</t>
         </is>
       </c>
     </row>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>['site_20', 'site_11', 'site_11']</t>
+          <t>['site_20', 'site_11']</t>
         </is>
       </c>
     </row>
@@ -2026,12 +2026,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox']</t>
+          <t>['iron/sulfur_redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['arginine and proline', 'amino acid related enzymes']</t>
+          <t>['amino acid related enzymes', 'arginine and proline']</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -2256,7 +2256,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox']</t>
+          <t>['electron transfer &amp; redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'direct_eet']</t>
+          <t>['direct_eet', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -2302,12 +2302,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>['one carbon pool by folate, cobalamin transport and', 'cysteine and methionine', 'selenocompound']</t>
+          <t>['one carbon pool by folate, cobalamin transport and', 'selenocompound', 'cysteine and methionine']</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -2394,12 +2394,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>['butanoate', 'valine, leucine and isoleucine degradation']</t>
+          <t>['valine, leucine and isoleucine degradation', 'butanoate']</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -2440,12 +2440,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['Viral proteins [BR:ko03200]', 'Messenger RNA biogenesis [BR:ko03019]']</t>
+          <t>['Messenger RNA biogenesis [BR:ko03019]', 'Viral proteins [BR:ko03200]']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'direct_eet', 'indirect_eet']</t>
+          <t>['indirect_eet', 'direct_eet', 'sulfur_metabolism', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -2647,7 +2647,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -2670,12 +2670,12 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>['lipopolysaccharide biosynthesis', 'lipopolysaccharide biosynthesis proteins']</t>
+          <t>['lipopolysaccharide biosynthesis proteins', 'lipopolysaccharide biosynthesis']</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -2762,12 +2762,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>['Antimicrobial resistance genes [BR:ko01504]', 'Peptidoglycan biosynthesis and degradation proteins [BR:ko01011]', 'Peptidoglycan biosynthesis']</t>
+          <t>['Peptidoglycan biosynthesis', 'Peptidoglycan biosynthesis and degradation proteins [BR:ko01011]', 'Antimicrobial resistance genes [BR:ko01504]']</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2777,7 +2777,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox']</t>
+          <t>['electron transfer &amp; redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'direct_eet']</t>
+          <t>['direct_eet', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['site_5', 'site_5']</t>
+          <t>['site_5']</t>
         </is>
       </c>
     </row>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['site_11', 'site_11']</t>
+          <t>['site_11']</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>['teichoic acid biosynthesis', 'lipopolysaccharide biosynthesis proteins']</t>
+          <t>['lipopolysaccharide biosynthesis proteins', 'teichoic acid biosynthesis']</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -2946,12 +2946,12 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>['butanoate', 'alanine, aspartate and glutamate']</t>
+          <t>['alanine, aspartate and glutamate', 'butanoate']</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -2992,12 +2992,12 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>['cationic antimicrobial peptide (camp) resistance', 'biosynthesis of various nucleotide sugars']</t>
+          <t>['biosynthesis of various nucleotide sugars', 'cationic antimicrobial peptide (camp) resistance']</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'indirect_eet']</t>
+          <t>['indirect_eet', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'direct_eet', 'acid_production', 'indirect_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3283,7 +3283,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -3291,7 +3291,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['site_5', 'site_5']</t>
+          <t>['site_5']</t>
         </is>
       </c>
     </row>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -3406,12 +3406,12 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>['Chromosome and associated proteins [BR:ko03036]', 'Transfer RNA biogenesis [BR:ko03016]', 'Mitochondrial biogenesis [BR:ko03029]', 'Viral proteins [BR:ko03200]', 'Messenger RNA biogenesis [BR:ko03019]']</t>
+          <t>['Transfer RNA biogenesis [BR:ko03016]', 'Chromosome and associated proteins [BR:ko03036]', 'Mitochondrial biogenesis [BR:ko03029]', 'Messenger RNA biogenesis [BR:ko03019]', 'Viral proteins [BR:ko03200]']</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -3452,12 +3452,12 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>['c5-branched dibasic acid', 'glyoxylate and dicarboxylate', 'other carbon fixation pathways', 'methane']</t>
+          <t>['other carbon fixation pathways', 'methane', 'glyoxylate and dicarboxylate', 'c5-branched dibasic acid']</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet', 'carbon_metabolism']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'carbon_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -3498,7 +3498,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3513,7 +3513,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -3544,7 +3544,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'acid_production']</t>
+          <t>['iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production']</t>
+          <t>['sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['site_3', 'site_3']</t>
+          <t>['site_3']</t>
         </is>
       </c>
     </row>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox']</t>
+          <t>['electron transfer &amp; redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3605,7 +3605,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'direct_eet']</t>
+          <t>['direct_eet', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production']</t>
+          <t>['acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production']</t>
+          <t>['acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -3682,12 +3682,12 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>['Antimicrobial resistance genes [BR:ko01504]', 'Peptidoglycan biosynthesis and degradation proteins [BR:ko01011]', 'Peptidoglycan biosynthesis']</t>
+          <t>['Peptidoglycan biosynthesis', 'Peptidoglycan biosynthesis and degradation proteins [BR:ko01011]', 'Antimicrobial resistance genes [BR:ko01504]']</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -3774,7 +3774,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'direct_eet', 'acid_production']</t>
+          <t>['direct_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -3820,12 +3820,12 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>['Antimicrobial resistance genes [BR:ko01504]', 'Peptidoglycan biosynthesis and degradation proteins [BR:ko01011]', 'Peptidoglycan biosynthesis']</t>
+          <t>['Peptidoglycan biosynthesis', 'Peptidoglycan biosynthesis and degradation proteins [BR:ko01011]', 'Antimicrobial resistance genes [BR:ko01504]']</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -3912,7 +3912,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox']</t>
+          <t>['electron transfer &amp; redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'direct_eet']</t>
+          <t>['direct_eet', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -4004,12 +4004,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>['Viral proteins [BR:ko03200]', 'Viral fusion proteins [BR:ko03210]']</t>
+          <t>['Viral fusion proteins [BR:ko03210]', 'Viral proteins [BR:ko03200]']</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'direct_eet', 'acid_production']</t>
+          <t>['direct_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -4050,12 +4050,12 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>['Chromosome and associated proteins [BR:ko03036]', 'Protein phosphatases and associated proteins [BR:ko01009]', 'Viral proteins [BR:ko03200]', 'Exosome [BR:ko04147]', 'Protein kinases [BR:ko01001]', 'Membrane trafficking [BR:ko04131]']</t>
+          <t>['Membrane trafficking [BR:ko04131]', 'Chromosome and associated proteins [BR:ko03036]', 'Exosome [BR:ko04147]', 'Protein phosphatases and associated proteins [BR:ko01009]', 'Protein kinases [BR:ko01001]', 'Viral proteins [BR:ko03200]']</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -4096,7 +4096,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -4142,12 +4142,12 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>['two-component system', 'pentose and glucuronate interconversions']</t>
+          <t>['pentose and glucuronate interconversions', 'two-component system']</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -4326,12 +4326,12 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>['glycine, serine and threonine', 'phenylalanine', 'tryptophan', 'drug - cytochrome p450, alcoholism', 'isoquinoline alkaloid biosynthesis', 'arginine and proline', 'tyrosine', 'histidine']</t>
+          <t>['drug - cytochrome p450, alcoholism', 'histidine', 'arginine and proline', 'isoquinoline alkaloid biosynthesis', 'tryptophan', 'glycine, serine and threonine', 'tyrosine', 'phenylalanine']</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4387,7 +4387,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4433,7 +4433,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['site_1', 'site_1']</t>
+          <t>['site_1']</t>
         </is>
       </c>
     </row>
@@ -4464,12 +4464,12 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>['arginine and proline', 'Viral proteins [BR:ko03200]', 'amino acid related enzymes', 'Messenger RNA biogenesis [BR:ko03019]']</t>
+          <t>['Messenger RNA biogenesis [BR:ko03019]', 'amino acid related enzymes', 'arginine and proline', 'Viral proteins [BR:ko03200]']</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -4479,7 +4479,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -4525,7 +4525,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'o2_consumption', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -4571,7 +4571,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'o2_consumption', 'indirect_eet', 'nitrogen_metabolism', 'direct_eet']</t>
+          <t>['direct_eet', 'o2_consumption', 'indirect_eet', 'biofilm_formation', 'nitrogen_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -4579,7 +4579,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>['site_4', 'site_4']</t>
+          <t>['site_4']</t>
         </is>
       </c>
     </row>
@@ -4602,7 +4602,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -4648,12 +4648,12 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>['amino sugar and nucleotide sugar', 'biosynthesis of various nucleotide sugars']</t>
+          <t>['biosynthesis of various nucleotide sugars', 'amino sugar and nucleotide sugar']</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -4694,12 +4694,12 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>['Viral proteins [BR:ko03200]', 'Messenger RNA biogenesis [BR:ko03019]']</t>
+          <t>['Messenger RNA biogenesis [BR:ko03019]', 'Viral proteins [BR:ko03200]']</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -4740,7 +4740,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production']</t>
+          <t>['acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -4755,7 +4755,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production']</t>
+          <t>['acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I94" t="n">
@@ -4786,12 +4786,12 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>['c5-branched dibasic acid', 'glyoxylate and dicarboxylate', 'other carbon fixation pathways', 'methane']</t>
+          <t>['other carbon fixation pathways', 'methane', 'glyoxylate and dicarboxylate', 'c5-branched dibasic acid']</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet', 'carbon_metabolism']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'carbon_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -4847,7 +4847,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet']</t>
+          <t>['indirect_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'electron transfer &amp; redox']</t>
+          <t>['electron transfer &amp; redox', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'direct_eet']</t>
+          <t>['direct_eet', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I97" t="n">
@@ -4924,12 +4924,12 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>['lipid biosynthesis proteins', 'butanoate']</t>
+          <t>['butanoate', 'lipid biosynthesis proteins']</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -4939,7 +4939,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I98" t="n">
@@ -4970,7 +4970,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -4985,7 +4985,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I99" t="n">
@@ -5016,7 +5016,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'iron/sulfur_redox', 'electron transfer &amp; redox', 'acid_production']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'indirect_eet', 'direct_eet', 'carbon_metabolism']</t>
+          <t>['direct_eet', 'indirect_eet', 'carbon_metabolism', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I100" t="n">
@@ -5062,7 +5062,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production', 'biofilm_formation', 'electron transfer &amp; redox', 'iron/sulfur_redox']</t>
+          <t>['electron transfer &amp; redox', 'iron/sulfur_redox', 'biofilm_formation', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -5077,7 +5077,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>['sulfur_metabolism', 'h2_consumption', 'acid_production', 'biofilm_formation', 'indirect_eet', 'direct_eet']</t>
+          <t>['direct_eet', 'indirect_eet', 'biofilm_formation', 'sulfur_metabolism', 'acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I101" t="n">
@@ -28585,7 +28585,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>['site_4', 'site_11', 'site_11', 'site_12', 'site_13']</t>
+          <t>['site_4', 'site_11', 'site_12', 'site_13']</t>
         </is>
       </c>
     </row>
@@ -28652,7 +28652,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>['site_4', 'site_11', 'site_11', 'site_12', 'site_13']</t>
+          <t>['site_4', 'site_11', 'site_12', 'site_13']</t>
         </is>
       </c>
     </row>
@@ -28719,7 +28719,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>['site_4', 'site_11', 'site_11', 'site_12', 'site_13']</t>
+          <t>['site_4', 'site_11', 'site_12', 'site_13']</t>
         </is>
       </c>
     </row>
@@ -28786,7 +28786,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>['site_4', 'site_11', 'site_11', 'site_12', 'site_13']</t>
+          <t>['site_4', 'site_11', 'site_12', 'site_13']</t>
         </is>
       </c>
     </row>
@@ -28814,7 +28814,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['aminoacyl-trna biosynthesis', 'mitochondrial biogenesis']</t>
+          <t>['mitochondrial biogenesis', 'aminoacyl-trna biosynthesis']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -28824,7 +28824,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['h2_consumption', 'acid_production']</t>
+          <t>['acid_production', 'h2_consumption']</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -28853,7 +28853,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>['site_4', 'site_11', 'site_11', 'site_12', 'site_13']</t>
+          <t>['site_4', 'site_11', 'site_12', 'site_13']</t>
         </is>
       </c>
     </row>

</xml_diff>